<commit_message>
update golang and openvswitch depend
</commit_message>
<xml_diff>
--- a/RPM_Dependency_Analysis.xlsx
+++ b/RPM_Dependency_Analysis.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="python-keystoneauth1" sheetId="1" r:id="rId1"/>
     <sheet name="systemd" sheetId="2" r:id="rId2"/>
     <sheet name="rabbitmq-server" sheetId="3" r:id="rId3"/>
+    <sheet name="openvswitch" sheetId="4" r:id="rId4"/>
+    <sheet name="golang" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="227">
   <si>
     <t>python3-betamax srpm-&gt;rpm</t>
   </si>
@@ -346,6 +348,357 @@
   </si>
   <si>
     <t>texlive-latex</t>
+  </si>
+  <si>
+    <t>openvswitch</t>
+  </si>
+  <si>
+    <t>python3-sphinx</t>
+  </si>
+  <si>
+    <t>environment-modules</t>
+  </si>
+  <si>
+    <t>tcl</t>
+  </si>
+  <si>
+    <t>man-db</t>
+  </si>
+  <si>
+    <t>libpipeline</t>
+  </si>
+  <si>
+    <t>python3-requests-2.20.0-1.el8.noarch</t>
+  </si>
+  <si>
+    <t>python3-urllib3</t>
+  </si>
+  <si>
+    <t>python3-pysocks</t>
+  </si>
+  <si>
+    <t>python3-chardet</t>
+  </si>
+  <si>
+    <t>python3-babel</t>
+  </si>
+  <si>
+    <t>python3-pytz</t>
+  </si>
+  <si>
+    <t>python3-imagesize</t>
+  </si>
+  <si>
+    <t>python3-jinja2</t>
+  </si>
+  <si>
+    <t>python3-markupsafe</t>
+  </si>
+  <si>
+    <t>python3-packaging</t>
+  </si>
+  <si>
+    <t>python3-pygments</t>
+  </si>
+  <si>
+    <t>python3-snowballstemmer</t>
+  </si>
+  <si>
+    <t>python3-sphinx-theme-alabaster</t>
+  </si>
+  <si>
+    <t>python3-sphinxcontrib-websupport</t>
+  </si>
+  <si>
+    <t>python3-sqlalchemy</t>
+  </si>
+  <si>
+    <t>python3-whoosh</t>
+  </si>
+  <si>
+    <t>python3-sphinx_rtd_theme</t>
+  </si>
+  <si>
+    <t>fontawesome-fonts</t>
+  </si>
+  <si>
+    <t>fontawesome-fonts-web</t>
+  </si>
+  <si>
+    <t>lato-fonts</t>
+  </si>
+  <si>
+    <t>google-roboto-slab-fonts</t>
+  </si>
+  <si>
+    <t>python-sphinx-locale = 1:1.7.6-1.el8</t>
+  </si>
+  <si>
+    <t>python3-pyOpenSSL-18.0.0-1.el8.noarch</t>
+  </si>
+  <si>
+    <t>python3-cryptography &gt;= 2.2.1</t>
+  </si>
+  <si>
+    <t>python3-asn1crypto &gt;= 0.21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python3-idna &gt;= 2.1 </t>
+  </si>
+  <si>
+    <t>python3-cffi &gt;= 1.7</t>
+  </si>
+  <si>
+    <t>python3-pycparser</t>
+  </si>
+  <si>
+    <t>python3-ply = 3.11</t>
+  </si>
+  <si>
+    <t>rdma-core-devel</t>
+  </si>
+  <si>
+    <t>rdma-core</t>
+  </si>
+  <si>
+    <t>dracut</t>
+  </si>
+  <si>
+    <t>systemd-udev &gt;= 219</t>
+  </si>
+  <si>
+    <t>libibumad</t>
+  </si>
+  <si>
+    <t>librdmacm</t>
+  </si>
+  <si>
+    <t>libibverbs = 22-2.el8</t>
+  </si>
+  <si>
+    <t>libnl3</t>
+  </si>
+  <si>
+    <t>libmnl-devel</t>
+  </si>
+  <si>
+    <t>libmnl</t>
+  </si>
+  <si>
+    <t>libpcap-devel</t>
+  </si>
+  <si>
+    <t>libpcap</t>
+  </si>
+  <si>
+    <t>golang</t>
+  </si>
+  <si>
+    <t>perl</t>
+  </si>
+  <si>
+    <t>perl-Archive-Tar</t>
+  </si>
+  <si>
+    <t>perl-Attribute-Handlers</t>
+  </si>
+  <si>
+    <t>perl-B-Debug</t>
+  </si>
+  <si>
+    <t>perl-CPAN</t>
+  </si>
+  <si>
+    <t>perl-CPAN-Meta</t>
+  </si>
+  <si>
+    <t>perl-CPAN-Meta-Requirements</t>
+  </si>
+  <si>
+    <t>perl-CPAN-Meta-YAML</t>
+  </si>
+  <si>
+    <t>perl-Compress-Raw-Bzip2</t>
+  </si>
+  <si>
+    <t>perl-Compress-Raw-Zlib</t>
+  </si>
+  <si>
+    <t>perl-Config-Perl-V</t>
+  </si>
+  <si>
+    <t>perl-DB_File</t>
+  </si>
+  <si>
+    <t>perl-Devel-PPPort</t>
+  </si>
+  <si>
+    <t>perl-Devel-Peek</t>
+  </si>
+  <si>
+    <t>perl-Devel-SelfStubber</t>
+  </si>
+  <si>
+    <t>perl-Digest</t>
+  </si>
+  <si>
+    <t>perl-Digest-MD5</t>
+  </si>
+  <si>
+    <t>perl-Digest-SHA</t>
+  </si>
+  <si>
+    <t>perl-Encode-devel</t>
+  </si>
+  <si>
+    <t>perl-Env</t>
+  </si>
+  <si>
+    <t>perl-ExtUtils-CBuilder</t>
+  </si>
+  <si>
+    <t>perl-ExtUtils-Miniperl</t>
+  </si>
+  <si>
+    <t>perl-File-Fetch</t>
+  </si>
+  <si>
+    <t>perl-Filter</t>
+  </si>
+  <si>
+    <t>perl-Filter-Simple</t>
+  </si>
+  <si>
+    <t>perl-IO-Compress</t>
+  </si>
+  <si>
+    <t>perl-IO-Socket-IP</t>
+  </si>
+  <si>
+    <t>perl-IO-Zlib</t>
+  </si>
+  <si>
+    <t>perl-IPC-Cmd</t>
+  </si>
+  <si>
+    <t>perl-IPC-SysV</t>
+  </si>
+  <si>
+    <t>perl-JSON-PP</t>
+  </si>
+  <si>
+    <t>perl-Locale-Codes</t>
+  </si>
+  <si>
+    <t>perl-Locale-Maketext</t>
+  </si>
+  <si>
+    <t>perl-Locale-Maketext-Simple</t>
+  </si>
+  <si>
+    <t>perl-Math-BigInt</t>
+  </si>
+  <si>
+    <t>perl-Math-BigInt-FastCalc</t>
+  </si>
+  <si>
+    <t>perl-Math-BigRat</t>
+  </si>
+  <si>
+    <t>perl-Math-Complex</t>
+  </si>
+  <si>
+    <t>perl-Memoize</t>
+  </si>
+  <si>
+    <t>perl-Module-CoreList</t>
+  </si>
+  <si>
+    <t>perl-Module-CoreList-tools</t>
+  </si>
+  <si>
+    <t>perl-Module-Load</t>
+  </si>
+  <si>
+    <t>perl-Module-Load-Conditional</t>
+  </si>
+  <si>
+    <t>perl-Module-Loaded</t>
+  </si>
+  <si>
+    <t>perl-Module-Metadata</t>
+  </si>
+  <si>
+    <t>perl-Net-Ping</t>
+  </si>
+  <si>
+    <t>perl-Params-Check</t>
+  </si>
+  <si>
+    <t>perl-Perl-OSType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perl-PerlIO-via-QuotedPrint </t>
+  </si>
+  <si>
+    <t xml:space="preserve">perl-Pod-Checker </t>
+  </si>
+  <si>
+    <t xml:space="preserve">perl-Pod-Html </t>
+  </si>
+  <si>
+    <t>perl-Pod-Parser</t>
+  </si>
+  <si>
+    <t>perl-SelfLoader</t>
+  </si>
+  <si>
+    <t>perl-Sys-Syslog</t>
+  </si>
+  <si>
+    <t>perl-Test</t>
+  </si>
+  <si>
+    <t>perl-Test-Simple</t>
+  </si>
+  <si>
+    <t>perl-Text-Balanced</t>
+  </si>
+  <si>
+    <t>perl-Time-HiRes</t>
+  </si>
+  <si>
+    <t>perl-Time-Piece</t>
+  </si>
+  <si>
+    <t>perl-Unicode-Collate</t>
+  </si>
+  <si>
+    <t>perl-autodie</t>
+  </si>
+  <si>
+    <t>perl-bignum</t>
+  </si>
+  <si>
+    <t>perl-encoding</t>
+  </si>
+  <si>
+    <t>perl-experimental</t>
+  </si>
+  <si>
+    <t>perl-libnet</t>
+  </si>
+  <si>
+    <t>perl-libnetcfg</t>
+  </si>
+  <si>
+    <t>perl-open</t>
+  </si>
+  <si>
+    <t>perl-perlfaq</t>
+  </si>
+  <si>
+    <t>perl-utils</t>
   </si>
 </sst>
 </file>
@@ -417,7 +770,297 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="40">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="9" tint="-0.24994659260841701"/>
@@ -821,7 +1464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -1284,12 +1927,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B100">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="python3-">
+    <cfRule type="containsText" dxfId="39" priority="11" operator="containsText" text="python3-">
       <formula>NOT(ISERROR(SEARCH("python3-",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D112">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="python3">
+    <cfRule type="containsText" dxfId="38" priority="10" operator="containsText" text="python3">
       <formula>NOT(ISERROR(SEARCH("python3",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1587,7 +2230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -1671,4 +2314,703 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F53"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E37" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F38" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1:B55">
+    <cfRule type="uniqueValues" dxfId="13" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C53">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="l">
+      <formula>NOT(ISERROR(SEARCH("l",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D53">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="l">
+      <formula>NOT(ISERROR(SEARCH("l",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="d">
+      <formula>NOT(ISERROR(SEARCH("d",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{3B5A8E3B-DCEE-4099-84AB-C19388EECD1B}">
+            <xm:f>NOT(ISERROR(SEARCH("-",C1)))</xm:f>
+            <xm:f>"-"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C6500"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFEB9C"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C1:C54</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{37AA0ECF-121E-427A-8DE7-A7BD55B8F209}">
+            <xm:f>NOT(ISERROR(SEARCH("-",D1)))</xm:f>
+            <xm:f>"-"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D1:D53</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{8107C95A-3B5A-4965-8149-D73FF05D4740}">
+            <xm:f>NOT(ISERROR(SEARCH("-",E1)))</xm:f>
+            <xm:f>"-"</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="4" tint="-0.24994659260841701"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor theme="3" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E1:E53</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G82" sqref="G82"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>226</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1:B74">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="perl">
+      <formula>NOT(ISERROR(SEARCH("perl",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update RPM dependency list
add resource-agents-4.1.1-12.el7_6.7.src.rpm dependency

Signed-off-by: LongLi <lilong-neu@neusoft.com>
</commit_message>
<xml_diff>
--- a/RPM_Dependency_Analysis.xlsx
+++ b/RPM_Dependency_Analysis.xlsx
@@ -12,13 +12,14 @@
     <sheet name="rabbitmq-server" sheetId="3" r:id="rId3"/>
     <sheet name="openvswitch" sheetId="4" r:id="rId4"/>
     <sheet name="golang" sheetId="5" r:id="rId5"/>
+    <sheet name="resource-agents" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="257">
   <si>
     <t>python3-betamax srpm-&gt;rpm</t>
   </si>
@@ -699,6 +700,96 @@
   </si>
   <si>
     <t>perl-utils</t>
+  </si>
+  <si>
+    <t>resource-agents</t>
+  </si>
+  <si>
+    <t>python3-setuptools-39.2.0-4.el8.noarch.rpm</t>
+  </si>
+  <si>
+    <t>perl-4:5.26.3-416.el8.x86_64</t>
+  </si>
+  <si>
+    <t>perl(Text::Diff)</t>
+  </si>
+  <si>
+    <t>perl-Algorithm-Diff-1.1903-9.el8.noarch.rpm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perl(Compress::Bzip2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">perl(Devel::Size) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">perl(Module::Build) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">perl(Text::Glob) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">perl(URI) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">perl(URI::Escape) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">perl(local::lib) </t>
+  </si>
+  <si>
+    <t>perl(File::HomeDir) &gt;= 0.65</t>
+  </si>
+  <si>
+    <t>perl-File-Which-1.22-2.el8.noarch.rpm</t>
+  </si>
+  <si>
+    <t>perl-ExtUtils-MM-Utils-7.34-1.el8.noarch.rpm</t>
+  </si>
+  <si>
+    <t>perl-Module-Build-0.42.24-5.el8.noarch.rpm</t>
+  </si>
+  <si>
+    <t>perl-Software-License-0.103013-2.el8.noarch.rpm</t>
+  </si>
+  <si>
+    <t>perl-Data-Section-0.200007-3.el8.noarch.rpm</t>
+  </si>
+  <si>
+    <t>perl-Sub-Exporter-0.987-15.el8.noarch.rpm</t>
+  </si>
+  <si>
+    <t>perl-Sub-Install-0.928-14.el8.noarch.rpm</t>
+  </si>
+  <si>
+    <t>perl-Params-Util-1.07-22.el8.x86_64.rpm</t>
+  </si>
+  <si>
+    <t>perl-Data-OptList-0.110-6.el8.noarch.rpm</t>
+  </si>
+  <si>
+    <t>perl-Package-Generator-1.106-11.el8.noarch.rpm</t>
+  </si>
+  <si>
+    <t>perl-MRO-Compat-0.13-4.el8.noarch.rpm</t>
+  </si>
+  <si>
+    <t>perl-Text-Template-1.51-1.el8.noarch.rpm</t>
+  </si>
+  <si>
+    <t>perl-inc-latest-0.500-9.el8.noarch.rpm</t>
+  </si>
+  <si>
+    <t>perl-PerlIO-via-QuotedPrint</t>
+  </si>
+  <si>
+    <t>perl-Pod-Checker</t>
+  </si>
+  <si>
+    <t>perl-Pod-Html</t>
+  </si>
+  <si>
+    <t>perl-IPC-System-Simple-1.25-17.el8.noarch.rpm</t>
   </si>
 </sst>
 </file>
@@ -770,7 +861,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="19">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -803,61 +894,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -888,166 +929,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1927,12 +1808,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B100">
-    <cfRule type="containsText" dxfId="39" priority="11" operator="containsText" text="python3-">
+    <cfRule type="containsText" dxfId="18" priority="11" operator="containsText" text="python3-">
       <formula>NOT(ISERROR(SEARCH("python3-",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D112">
-    <cfRule type="containsText" dxfId="38" priority="10" operator="containsText" text="python3">
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="python3">
       <formula>NOT(ISERROR(SEARCH("python3",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2568,18 +2449,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B55">
-    <cfRule type="uniqueValues" dxfId="13" priority="7"/>
+    <cfRule type="uniqueValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C53">
-    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="l">
+    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="l">
       <formula>NOT(ISERROR(SEARCH("l",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D53">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="l">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="l">
       <formula>NOT(ISERROR(SEARCH("l",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="d">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="d">
       <formula>NOT(ISERROR(SEARCH("d",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2650,7 +2531,7 @@
   <dimension ref="A1:B70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G82" sqref="G82"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3013,4 +2894,514 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G100"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="60" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="61" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="62" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D63" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E64" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="F65" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="G66" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="67" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="G67" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="G68" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="69" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="G69" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="71" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="F71" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="72" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="E72" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="73" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D73" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="74" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C74" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="75" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C75" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="76" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C76" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="77" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C77" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="78" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C78" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="79" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C79" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="80" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C80" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C81" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C82" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C83" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C84" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C85" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C86" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="87" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C87" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C88" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="89" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C89" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="90" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D90" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="91" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C91" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="92" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C92" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="93" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C93" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="94" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C94" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="95" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C95" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="96" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C96" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C97" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C98" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C99" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C100" t="s">
+        <v>255</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>